<commit_message>
Add Cart Valid and Invalid Features
</commit_message>
<xml_diff>
--- a/DummyJson API Testing.xlsx
+++ b/DummyJson API Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ousse\Desktop\Courses\DummyJson_API_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217856C7-9B4A-4240-99FE-6C73D5ECEB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C02F98-772D-4973-9266-68A779671221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -176,66 +176,12 @@
     <t>TC_10</t>
   </si>
   <si>
-    <t>Fetch Cart</t>
-  </si>
-  <si>
-    <t>Cart items for the user</t>
-  </si>
-  <si>
-    <t>1. Send a GET request to /carts/{userId} with a valid user ID. &lt;br&gt; 2. Receive a JSON response with the user's cart items.</t>
-  </si>
-  <si>
     <t>TC_11</t>
   </si>
   <si>
-    <t>1. Send a GET request to /carts/{userId} with an invalid user ID. &lt;br&gt; 2. Receive an error response with an appropriate error message.</t>
-  </si>
-  <si>
     <t>TC_12</t>
   </si>
   <si>
-    <t>Fetch Order List</t>
-  </si>
-  <si>
-    <t>List of orders for the user</t>
-  </si>
-  <si>
-    <t>1. Send a GET request to /orders/{userId} with a valid user ID. &lt;br&gt; 2. Receive a JSON response with a list of the user's orders.</t>
-  </si>
-  <si>
-    <t>TC_13</t>
-  </si>
-  <si>
-    <t>1. Send a GET request to /orders/{userId} with an invalid user ID. &lt;br&gt; 2. Receive an error response with an appropriate error message.</t>
-  </si>
-  <si>
-    <t>TC_14</t>
-  </si>
-  <si>
-    <t>Fetch Single Order</t>
-  </si>
-  <si>
-    <t>Valid order ID</t>
-  </si>
-  <si>
-    <t>Detailed order information</t>
-  </si>
-  <si>
-    <t>1. Send a GET request to /orders/{orderId} with a valid order ID. &lt;br&gt; 2. Receive a JSON response with detailed order information.</t>
-  </si>
-  <si>
-    <t>TC_15</t>
-  </si>
-  <si>
-    <t>Invalid order ID</t>
-  </si>
-  <si>
-    <t>Error message indicating order not found</t>
-  </si>
-  <si>
-    <t>1. Send a GET request to /orders/{orderId} with an invalid order ID. &lt;br&gt; 2. Receive an error response with an appropriate error message.</t>
-  </si>
-  <si>
     <t>TC_16</t>
   </si>
   <si>
@@ -342,6 +288,39 @@
   </si>
   <si>
     <t>1. Gradually increase the load on the API. &lt;br&gt; 2. Monitor the API's performance metrics (response time, throughput, error rate) under increasing load.</t>
+  </si>
+  <si>
+    <t>Fetch All Carts</t>
+  </si>
+  <si>
+    <t>All carts appears in response</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /carts. &lt;br&gt; 2. Receive a JSON response with all carts items.</t>
+  </si>
+  <si>
+    <t>Fetch Single Cart with ID</t>
+  </si>
+  <si>
+    <t>Valid Cart ID</t>
+  </si>
+  <si>
+    <t>Single cart details appears in response</t>
+  </si>
+  <si>
+    <t>Fetch Invalid Single Cart with ID</t>
+  </si>
+  <si>
+    <t>Invalid Cart ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message and status code 404 </t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /carts/{cartID} with an valid cart ID. &lt;br&gt; 2.  Receive a JSON response with single Cart details</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /carts/{cartID} with an invalid cart ID. &lt;br&gt; 2.  Receive an error message.</t>
   </si>
 </sst>
 </file>
@@ -879,135 +858,109 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" customWidth="1"/>
+    <col min="7" max="7" width="103.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1021,9 +974,15 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1050,87 +1009,87 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1174,53 +1133,53 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Readme.MD and POJO classes
</commit_message>
<xml_diff>
--- a/DummyJson API Testing.xlsx
+++ b/DummyJson API Testing.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ousse\Desktop\Courses\DummyJson_API_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B98805B-06AB-447B-AC36-255EEBB06C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C399017-705F-4AA6-A78F-7D14E78D128F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="756" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="756" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Data Retrieval" sheetId="1" r:id="rId1"/>
     <sheet name="User Data Retrieval" sheetId="2" r:id="rId2"/>
-    <sheet name="Cart and Order Data Retrieval" sheetId="3" r:id="rId3"/>
+    <sheet name="Cart Data Retrieval" sheetId="3" r:id="rId3"/>
     <sheet name="Recipe Data Retrieval" sheetId="6" r:id="rId4"/>
     <sheet name="Error Handling and Validation" sheetId="4" r:id="rId5"/>
     <sheet name="Performance Tests" sheetId="5" r:id="rId6"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="111">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -150,9 +150,6 @@
     <t>TC_08</t>
   </si>
   <si>
-    <t>Fetch Single User</t>
-  </si>
-  <si>
     <t>Valid user ID</t>
   </si>
   <si>
@@ -355,6 +352,12 @@
   </si>
   <si>
     <t>1. Send a GET request to /recipes/{recipeID} with an invalid cart ID. &lt;br&gt; 2.  Receive an error message.</t>
+  </si>
+  <si>
+    <t>Fetch Valid Single User</t>
+  </si>
+  <si>
+    <t>Fetch Invalid Single User</t>
   </si>
 </sst>
 </file>
@@ -796,8 +799,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -850,33 +853,33 @@
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +895,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -929,51 +932,51 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -989,7 +992,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1009,7 +1012,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1047,51 +1050,51 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1141,87 +1144,87 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1239,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -1267,53 +1270,53 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cart retrieval test case in Readme.md file
</commit_message>
<xml_diff>
--- a/DummyJson API Testing.xlsx
+++ b/DummyJson API Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ousse\Desktop\Courses\DummyJson_API_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C399017-705F-4AA6-A78F-7D14E78D128F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED19E2E-9C71-4009-8B9F-18B64A69EC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="756" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="756" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Data Retrieval" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>1. Send a GET request to /recipes. &lt;br&gt; 2. Receive a JSON response with all carts items.</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>Fetch Single Recipe with ID</t>
@@ -799,7 +796,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -853,7 +850,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>41</v>
@@ -870,7 +867,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>45</v>
@@ -894,8 +891,8 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -991,9 +988,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -1068,16 +1063,16 @@
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>92</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1085,16 +1080,16 @@
         <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>95</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Invalid User Login Scenario
</commit_message>
<xml_diff>
--- a/DummyJson API Testing.xlsx
+++ b/DummyJson API Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ousse\Desktop\Courses\DummyJson_API_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED19E2E-9C71-4009-8B9F-18B64A69EC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752EB4B1-99BD-4656-BF0D-083B62D92797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="756" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="756" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Data Retrieval" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Fetch Invalid Single User</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>TC_15</t>
   </si>
 </sst>
 </file>
@@ -891,7 +897,7 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1007,7 +1013,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1066,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>102</v>
@@ -1077,7 +1083,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>104</v>
@@ -1234,8 +1240,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>